<commit_message>
deltaT vs. emissions graph
</commit_message>
<xml_diff>
--- a/chapters/ch02-Boundaries/datasets/SPM_10.xlsx
+++ b/chapters/ch02-Boundaries/datasets/SPM_10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch02-Boundaries/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{97AB71DF-17D4-864A-8D65-150EE6BA3631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{93F4DA7B-69A2-1F4E-980A-17905E238853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="23">
   <si>
     <t>Cumulative CO2 emissions since 1850</t>
   </si>
@@ -65,24 +65,6 @@
     <t>dataset</t>
   </si>
   <si>
-    <t>history</t>
-  </si>
-  <si>
-    <t>SSP1-19</t>
-  </si>
-  <si>
-    <t>SSP1-26</t>
-  </si>
-  <si>
-    <t>SSP2-45</t>
-  </si>
-  <si>
-    <t>SSP3-70</t>
-  </si>
-  <si>
-    <t>SSP5-85</t>
-  </si>
-  <si>
     <t>Data are from this figure</t>
   </si>
   <si>
@@ -96,6 +78,24 @@
   </si>
   <si>
     <t>https://www.ipcc.ch/report/ar6/wg1/#InteractiveAtlas</t>
+  </si>
+  <si>
+    <t>Historical</t>
+  </si>
+  <si>
+    <t>SSP1-1.9</t>
+  </si>
+  <si>
+    <t>SSP1-2.6</t>
+  </si>
+  <si>
+    <t>SSP2-4.5</t>
+  </si>
+  <si>
+    <t>SSP3-7.0</t>
+  </si>
+  <si>
+    <t>SSP5-8.5</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C351"/>
+  <dimension ref="A1:C326"/>
   <sheetViews>
-    <sheetView topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="C351" sqref="C316:C351"/>
+    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="C296" sqref="C296:C326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1111,7 +1111,7 @@
         <v>-5.8676470588235302E-2</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1122,7 +1122,7 @@
         <v>4.8823529411764703E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1133,7 +1133,7 @@
         <v>7.8823529411764695E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1144,7 +1144,7 @@
         <v>4.6323529411764701E-2</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1155,7 +1155,7 @@
         <v>4.8823529411764703E-2</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1166,7 +1166,7 @@
         <v>4.8823529411764703E-2</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1177,7 +1177,7 @@
         <v>-5.1176470588235302E-2</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
         <v>-0.14617647058823499</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1199,7 +1199,7 @@
         <v>-3.8676470588235298E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>6.88235294117647E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1221,7 +1221,7 @@
         <v>-5.61764705882353E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1232,7 +1232,7 @@
         <v>-9.1176470588235303E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1243,7 +1243,7 @@
         <v>-0.153676470588235</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1254,7 +1254,7 @@
         <v>1.3235294117647199E-3</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>-4.86764705882353E-2</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
         <v>3.3823529411764697E-2</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1287,7 +1287,7 @@
         <v>5.1323529411764698E-2</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1298,7 +1298,7 @@
         <v>4.8823529411764703E-2</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
         <v>6.13235294117647E-2</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1320,7 +1320,7 @@
         <v>5.8823529411764698E-2</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1331,7 +1331,7 @@
         <v>2.13235294117647E-2</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1342,7 +1342,7 @@
         <v>-6.1764705882352599E-3</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1353,7 +1353,7 @@
         <v>2.3823529411764698E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1364,7 +1364,7 @@
         <v>1.6323529411764699E-2</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1375,7 +1375,7 @@
         <v>-2.11764705882353E-2</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1386,7 +1386,7 @@
         <v>-6.1764705882352703E-3</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1397,7 +1397,7 @@
         <v>-4.3676470588235303E-2</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1408,7 +1408,7 @@
         <v>0.27132352941176502</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1419,7 +1419,7 @@
         <v>0.33132352941176502</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1430,7 +1430,7 @@
         <v>8.38235294117647E-2</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1441,7 +1441,7 @@
         <v>3.1323529411764701E-2</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1452,7 +1452,7 @@
         <v>0.11632352941176501</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1463,7 +1463,7 @@
         <v>6.3823529411764807E-2</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1474,7 +1474,7 @@
         <v>-1.1764705882352699E-3</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1485,7 +1485,7 @@
         <v>-0.128676470588235</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1496,7 +1496,7 @@
         <v>-0.13367647058823501</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1507,7 +1507,7 @@
         <v>-0.113676470588235</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1518,7 +1518,7 @@
         <v>-0.16867647058823501</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1529,7 +1529,7 @@
         <v>-1.11764705882353E-2</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1540,7 +1540,7 @@
         <v>0.111323529411765</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1551,7 +1551,7 @@
         <v>-0.14617647058823499</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1562,7 +1562,7 @@
         <v>-3.8676470588235298E-2</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1573,7 +1573,7 @@
         <v>-0.121176470588235</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1584,7 +1584,7 @@
         <v>-0.11867647058823499</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1595,7 +1595,7 @@
         <v>-0.10117647058823501</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1606,7 +1606,7 @@
         <v>-5.8676470588235302E-2</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1617,7 +1617,7 @@
         <v>8.8823529411764704E-2</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1628,7 +1628,7 @@
         <v>8.8823529411764704E-2</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1639,7 +1639,7 @@
         <v>-0.113676470588235</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1650,7 +1650,7 @@
         <v>1.6323529411764699E-2</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1661,7 +1661,7 @@
         <v>0.11632352941176501</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1672,7 +1672,7 @@
         <v>6.3823529411764696E-2</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1683,7 +1683,7 @@
         <v>-7.8676470588235306E-2</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1694,7 +1694,7 @@
         <v>-0.16867647058823501</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1705,7 +1705,7 @@
         <v>-0.23867647058823499</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1716,7 +1716,7 @@
         <v>-5.3676470588235298E-2</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1727,7 +1727,7 @@
         <v>2.3823529411764698E-2</v>
       </c>
       <c r="C58" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1738,7 +1738,7 @@
         <v>-0.13367647058823501</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1749,7 +1749,7 @@
         <v>-0.17367647058823499</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1760,7 +1760,7 @@
         <v>-0.221176470588235</v>
       </c>
       <c r="C61" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1771,7 +1771,7 @@
         <v>-0.191176470588235</v>
       </c>
       <c r="C62" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1782,7 +1782,7 @@
         <v>-0.20867647058823499</v>
       </c>
       <c r="C63" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1793,7 +1793,7 @@
         <v>-0.13617647058823501</v>
       </c>
       <c r="C64" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1804,7 +1804,7 @@
         <v>-0.113676470588235</v>
       </c>
       <c r="C65" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1815,7 +1815,7 @@
         <v>7.8823529411764695E-2</v>
       </c>
       <c r="C66" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1826,7 +1826,7 @@
         <v>0.13632352941176501</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1837,7 +1837,7 @@
         <v>-8.6176470588235299E-2</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1848,7 +1848,7 @@
         <v>-0.213676470588235</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1859,7 +1859,7 @@
         <v>-6.1176470588235297E-2</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1870,7 +1870,7 @@
         <v>-6.1764705882352798E-3</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1881,7 +1881,7 @@
         <v>3.3823529411764697E-2</v>
       </c>
       <c r="C72" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1892,7 +1892,7 @@
         <v>7.3823529411764802E-2</v>
       </c>
       <c r="C73" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1903,7 +1903,7 @@
         <v>-8.6764705882352907E-3</v>
       </c>
       <c r="C74" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1914,7 +1914,7 @@
         <v>1.6323529411764699E-2</v>
       </c>
       <c r="C75" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1925,7 +1925,7 @@
         <v>1.8823529411764701E-2</v>
       </c>
       <c r="C76" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1936,7 +1936,7 @@
         <v>5.6323529411764703E-2</v>
       </c>
       <c r="C77" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1947,7 +1947,7 @@
         <v>0.186323529411765</v>
       </c>
       <c r="C78" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1958,7 +1958,7 @@
         <v>8.1323529411764697E-2</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1969,7 +1969,7 @@
         <v>9.1323529411764706E-2</v>
       </c>
       <c r="C80" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1980,7 +1980,7 @@
         <v>-7.1176470588235299E-2</v>
       </c>
       <c r="C81" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1991,7 +1991,7 @@
         <v>0.13632352941176501</v>
       </c>
       <c r="C82" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2002,7 +2002,7 @@
         <v>0.19882352941176501</v>
       </c>
       <c r="C83" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2013,7 +2013,7 @@
         <v>0.153823529411765</v>
       </c>
       <c r="C84" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2024,7 +2024,7 @@
         <v>-1.11764705882353E-2</v>
       </c>
       <c r="C85" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2035,7 +2035,7 @@
         <v>0.13632352941176501</v>
       </c>
       <c r="C86" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2046,7 +2046,7 @@
         <v>8.8823529411764704E-2</v>
       </c>
       <c r="C87" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2057,7 +2057,7 @@
         <v>0.13632352941176501</v>
       </c>
       <c r="C88" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2068,7 +2068,7 @@
         <v>0.28382352941176497</v>
       </c>
       <c r="C89" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2079,7 +2079,7 @@
         <v>0.28632352941176498</v>
       </c>
       <c r="C90" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2090,7 +2090,7 @@
         <v>0.27132352941176502</v>
       </c>
       <c r="C91" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2101,7 +2101,7 @@
         <v>0.371323529411765</v>
       </c>
       <c r="C92" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2112,7 +2112,7 @@
         <v>0.35632352941176498</v>
       </c>
       <c r="C93" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2123,7 +2123,7 @@
         <v>0.32132352941176501</v>
       </c>
       <c r="C94" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2134,7 +2134,7 @@
         <v>0.34882352941176498</v>
       </c>
       <c r="C95" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2145,7 +2145,7 @@
         <v>0.47132352941176497</v>
       </c>
       <c r="C96" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2156,7 +2156,7 @@
         <v>0.34882352941176498</v>
       </c>
       <c r="C97" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2167,7 +2167,7 @@
         <v>0.19632352941176501</v>
       </c>
       <c r="C98" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2178,7 +2178,7 @@
         <v>0.24132352941176499</v>
       </c>
       <c r="C99" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2189,7 +2189,7 @@
         <v>0.18132352941176499</v>
       </c>
       <c r="C100" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2200,7 +2200,7 @@
         <v>0.17382352941176499</v>
       </c>
       <c r="C101" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -2211,7 +2211,7 @@
         <v>9.6323529411764697E-2</v>
       </c>
       <c r="C102" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -2222,7 +2222,7 @@
         <v>0.251323529411765</v>
       </c>
       <c r="C103" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -2233,7 +2233,7 @@
         <v>0.32382352941176501</v>
       </c>
       <c r="C104" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -2244,7 +2244,7 @@
         <v>0.38882352941176501</v>
       </c>
       <c r="C105" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -2255,7 +2255,7 @@
         <v>0.19632352941176501</v>
       </c>
       <c r="C106" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -2266,7 +2266,7 @@
         <v>0.13882352941176501</v>
       </c>
       <c r="C107" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -2277,7 +2277,7 @@
         <v>7.6323529411764707E-2</v>
       </c>
       <c r="C108" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2288,7 +2288,7 @@
         <v>0.29632352941176499</v>
       </c>
       <c r="C109" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -2299,7 +2299,7 @@
         <v>0.30632352941176499</v>
       </c>
       <c r="C110" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -2310,7 +2310,7 @@
         <v>0.28632352941176498</v>
       </c>
       <c r="C111" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2321,7 +2321,7 @@
         <v>0.23132352941176501</v>
       </c>
       <c r="C112" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -2332,7 +2332,7 @@
         <v>0.308823529411765</v>
       </c>
       <c r="C113" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -2343,7 +2343,7 @@
         <v>0.26132352941176501</v>
       </c>
       <c r="C114" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2354,7 +2354,7 @@
         <v>0.29632352941176499</v>
       </c>
       <c r="C115" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -2365,7 +2365,7 @@
         <v>4.6323529411764701E-2</v>
       </c>
       <c r="C116" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -2376,7 +2376,7 @@
         <v>0.153823529411765</v>
       </c>
       <c r="C117" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -2387,7 +2387,7 @@
         <v>0.20632352941176499</v>
       </c>
       <c r="C118" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -2398,7 +2398,7 @@
         <v>0.23882352941176499</v>
       </c>
       <c r="C119" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -2409,7 +2409,7 @@
         <v>0.17132352941176501</v>
       </c>
       <c r="C120" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -2420,7 +2420,7 @@
         <v>0.313823529411765</v>
       </c>
       <c r="C121" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -2431,7 +2431,7 @@
         <v>0.27382352941176502</v>
       </c>
       <c r="C122" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -2442,7 +2442,7 @@
         <v>0.153823529411765</v>
       </c>
       <c r="C123" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -2453,7 +2453,7 @@
         <v>0.26132352941176501</v>
       </c>
       <c r="C124" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -2464,7 +2464,7 @@
         <v>0.40382352941176503</v>
       </c>
       <c r="C125" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -2475,7 +2475,7 @@
         <v>0.183823529411765</v>
       </c>
       <c r="C126" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -2486,7 +2486,7 @@
         <v>0.24132352941176499</v>
       </c>
       <c r="C127" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -2497,7 +2497,7 @@
         <v>0.14882352941176499</v>
       </c>
       <c r="C128" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -2508,7 +2508,7 @@
         <v>0.45382352941176501</v>
       </c>
       <c r="C129" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -2519,7 +2519,7 @@
         <v>0.34882352941176498</v>
       </c>
       <c r="C130" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -2530,7 +2530,7 @@
         <v>0.436323529411765</v>
       </c>
       <c r="C131" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -2541,7 +2541,7 @@
         <v>0.54132352941176498</v>
       </c>
       <c r="C132" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -2552,7 +2552,7 @@
         <v>0.58632352941176502</v>
       </c>
       <c r="C133" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -2563,7 +2563,7 @@
         <v>0.39632352941176502</v>
       </c>
       <c r="C134" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -2574,7 +2574,7 @@
         <v>0.57132352941176501</v>
       </c>
       <c r="C135" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -2585,7 +2585,7 @@
         <v>0.40882352941176497</v>
       </c>
       <c r="C136" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -2596,7 +2596,7 @@
         <v>0.40132352941176502</v>
       </c>
       <c r="C137" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -2607,7 +2607,7 @@
         <v>0.441323529411765</v>
       </c>
       <c r="C138" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -2618,7 +2618,7 @@
         <v>0.57882352941176496</v>
       </c>
       <c r="C139" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -2629,7 +2629,7 @@
         <v>0.63382352941176501</v>
       </c>
       <c r="C140" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -2640,7 +2640,7 @@
         <v>0.52382352941176502</v>
       </c>
       <c r="C141" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -2651,7 +2651,7 @@
         <v>0.69882352941176495</v>
       </c>
       <c r="C142" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -2662,7 +2662,7 @@
         <v>0.67632352941176499</v>
       </c>
       <c r="C143" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -2673,7 +2673,7 @@
         <v>0.47382352941176498</v>
       </c>
       <c r="C144" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -2684,7 +2684,7 @@
         <v>0.52132352941176496</v>
       </c>
       <c r="C145" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -2695,7 +2695,7 @@
         <v>0.57632352941176501</v>
       </c>
       <c r="C146" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -2706,7 +2706,7 @@
         <v>0.72632352941176503</v>
       </c>
       <c r="C147" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -2717,7 +2717,7 @@
         <v>0.61382352941176499</v>
       </c>
       <c r="C148" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -2728,7 +2728,7 @@
         <v>0.75882352941176501</v>
       </c>
       <c r="C149" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -2739,7 +2739,7 @@
         <v>0.90132352941176497</v>
       </c>
       <c r="C150" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -2750,7 +2750,7 @@
         <v>0.66632352941176498</v>
       </c>
       <c r="C151" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -2761,7 +2761,7 @@
         <v>0.66882352941176504</v>
       </c>
       <c r="C152" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -2772,7 +2772,7 @@
         <v>0.811323529411765</v>
       </c>
       <c r="C153" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -2783,7 +2783,7 @@
         <v>0.88132352941176495</v>
       </c>
       <c r="C154" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -2794,7 +2794,7 @@
         <v>0.878823529411765</v>
       </c>
       <c r="C155" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -2805,7 +2805,7 @@
         <v>0.80382352941176505</v>
       </c>
       <c r="C156" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -2816,7 +2816,7 @@
         <v>0.94382352941176495</v>
       </c>
       <c r="C157" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -2827,7 +2827,7 @@
         <v>0.90382352941176503</v>
       </c>
       <c r="C158" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -2838,7 +2838,7 @@
         <v>0.92132352941176499</v>
       </c>
       <c r="C159" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -2849,7 +2849,7 @@
         <v>0.79632352941176499</v>
       </c>
       <c r="C160" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -2860,7 +2860,7 @@
         <v>0.92632352941176499</v>
       </c>
       <c r="C161" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -2871,7 +2871,7 @@
         <v>0.99632352941176505</v>
       </c>
       <c r="C162" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -2882,7 +2882,7 @@
         <v>0.88132352941176495</v>
       </c>
       <c r="C163" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -2893,7 +2893,7 @@
         <v>0.90632352941176497</v>
       </c>
       <c r="C164" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
@@ -2904,7 +2904,7 @@
         <v>0.936323529411765</v>
       </c>
       <c r="C165" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
@@ -2915,7 +2915,7 @@
         <v>1.0063235294117601</v>
       </c>
       <c r="C166" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -2926,7 +2926,7 @@
         <v>1.1488235294117599</v>
       </c>
       <c r="C167" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
@@ -2937,7 +2937,7 @@
         <v>1.2638235294117599</v>
       </c>
       <c r="C168" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -2948,7 +2948,7 @@
         <v>1.1788235294117599</v>
       </c>
       <c r="C169" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
@@ -2959,7 +2959,7 @@
         <v>1.10132352941177</v>
       </c>
       <c r="C170" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -2970,1987 +2970,1712 @@
         <v>1.22632352941176</v>
       </c>
       <c r="C171" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172">
-        <v>2240.9857705551399</v>
+        <v>2438.3724025054398</v>
       </c>
       <c r="B172">
-        <v>1.07</v>
+        <v>1.1966657460730299</v>
       </c>
       <c r="C172" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173">
-        <v>2280.2466968835702</v>
+        <v>2476.3814834036898</v>
       </c>
       <c r="B173">
-        <v>1.0944269868869301</v>
+        <v>1.22290911532144</v>
       </c>
       <c r="C173" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174">
-        <v>2319.6158232428102</v>
+        <v>2512.7059187485202</v>
       </c>
       <c r="B174">
-        <v>1.12004905193271</v>
+        <v>1.2481523179237699</v>
       </c>
       <c r="C174" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175">
-        <v>2359.0931496328699</v>
+        <v>2547.34570853992</v>
       </c>
       <c r="B175">
-        <v>1.14639811271146</v>
+        <v>1.27123565389639</v>
       </c>
       <c r="C175" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176">
-        <v>2398.6786760537502</v>
+        <v>2580.3008527778902</v>
       </c>
       <c r="B176">
-        <v>1.17179686982236</v>
+        <v>1.29264797338667</v>
       </c>
       <c r="C176" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177">
-        <v>2438.3724025054398</v>
+        <v>2611.5713514624299</v>
       </c>
       <c r="B177">
-        <v>1.1966657460730299</v>
+        <v>1.3150223766909901</v>
       </c>
       <c r="C177" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178">
-        <v>2476.3814834036898</v>
+        <v>2641.15720459354</v>
       </c>
       <c r="B178">
-        <v>1.22290911532144</v>
+        <v>1.3379460343432299</v>
       </c>
       <c r="C178" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179">
-        <v>2512.7059187485202</v>
+        <v>2669.05841217123</v>
       </c>
       <c r="B179">
-        <v>1.2481523179237699</v>
+        <v>1.3594529407314699</v>
       </c>
       <c r="C179" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180">
-        <v>2547.34570853992</v>
+        <v>2695.2749741954799</v>
       </c>
       <c r="B180">
-        <v>1.27123565389639</v>
+        <v>1.37844996465023</v>
       </c>
       <c r="C180" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181">
-        <v>2580.3008527778902</v>
+        <v>2719.8068906663002</v>
       </c>
       <c r="B181">
-        <v>1.29264797338667</v>
+        <v>1.3972430689848501</v>
       </c>
       <c r="C181" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182">
-        <v>2611.5713514624299</v>
+        <v>2742.6541615837</v>
       </c>
       <c r="B182">
-        <v>1.3150223766909901</v>
+        <v>1.4146959511086701</v>
       </c>
       <c r="C182" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183">
-        <v>2641.15720459354</v>
+        <v>2764.26421429129</v>
       </c>
       <c r="B183">
-        <v>1.3379460343432299</v>
+        <v>1.4302758531075399</v>
       </c>
       <c r="C183" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184">
-        <v>2669.05841217123</v>
+        <v>2784.6370487890799</v>
       </c>
       <c r="B184">
-        <v>1.3594529407314699</v>
+        <v>1.44524629442606</v>
       </c>
       <c r="C184" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185">
-        <v>2695.2749741954799</v>
+        <v>2803.7726650770701</v>
       </c>
       <c r="B185">
-        <v>1.37844996465023</v>
+        <v>1.4590544570202499</v>
       </c>
       <c r="C185" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186">
-        <v>2719.8068906663002</v>
+        <v>2821.6710631552601</v>
       </c>
       <c r="B186">
-        <v>1.3972430689848501</v>
+        <v>1.47055267087258</v>
       </c>
       <c r="C186" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187">
-        <v>2742.6541615837</v>
+        <v>2838.3322430236399</v>
       </c>
       <c r="B187">
-        <v>1.4146959511086701</v>
+        <v>1.4812603627735299</v>
       </c>
       <c r="C187" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188">
-        <v>2764.26421429129</v>
+        <v>2853.75620468223</v>
       </c>
       <c r="B188">
-        <v>1.4302758531075399</v>
+        <v>1.49123947324701</v>
       </c>
       <c r="C188" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189">
-        <v>2784.6370487890799</v>
+        <v>2867.9429481310099</v>
       </c>
       <c r="B189">
-        <v>1.44524629442606</v>
+        <v>1.4994343893511</v>
       </c>
       <c r="C189" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190">
-        <v>2803.7726650770701</v>
+        <v>2880.8924733699901</v>
       </c>
       <c r="B190">
-        <v>1.4590544570202499</v>
+        <v>1.50652930675932</v>
       </c>
       <c r="C190" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191">
-        <v>2821.6710631552601</v>
+        <v>2892.6047803991701</v>
       </c>
       <c r="B191">
-        <v>1.47055267087258</v>
+        <v>1.5142626826861401</v>
       </c>
       <c r="C191" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192">
-        <v>2838.3322430236399</v>
+        <v>2903.0798692185499</v>
       </c>
       <c r="B192">
-        <v>1.4812603627735299</v>
+        <v>1.5208283413202801</v>
       </c>
       <c r="C192" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193">
-        <v>2853.75620468223</v>
+        <v>2912.7124853117698</v>
       </c>
       <c r="B193">
-        <v>1.49123947324701</v>
+        <v>1.5253147525071999</v>
       </c>
       <c r="C193" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194">
-        <v>2867.9429481310099</v>
+        <v>2921.5026286788202</v>
       </c>
       <c r="B194">
-        <v>1.4994343893511</v>
+        <v>1.5299278381281101</v>
       </c>
       <c r="C194" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195">
-        <v>2880.8924733699901</v>
+        <v>2929.4502993197102</v>
       </c>
       <c r="B195">
-        <v>1.50652930675932</v>
+        <v>1.53399372646951</v>
       </c>
       <c r="C195" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196">
-        <v>2892.6047803991701</v>
+        <v>2936.5554972344498</v>
       </c>
       <c r="B196">
-        <v>1.5142626826861401</v>
+        <v>1.53755018343668</v>
       </c>
       <c r="C196" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197">
-        <v>2903.0798692185499</v>
+        <v>2942.81822242301</v>
       </c>
       <c r="B197">
-        <v>1.5208283413202801</v>
+        <v>1.53931438168743</v>
       </c>
       <c r="C197" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198">
-        <v>2912.7124853117698</v>
+        <v>2948.2384748854201</v>
       </c>
       <c r="B198">
-        <v>1.5253147525071999</v>
+        <v>1.53836170183641</v>
       </c>
       <c r="C198" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199">
-        <v>2921.5026286788202</v>
+        <v>2952.8162546216699</v>
       </c>
       <c r="B199">
-        <v>1.5299278381281101</v>
+        <v>1.5381936982922899</v>
       </c>
       <c r="C199" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200">
-        <v>2929.4502993197102</v>
+        <v>2956.5515616317498</v>
       </c>
       <c r="B200">
-        <v>1.53399372646951</v>
+        <v>1.5379618744082899</v>
       </c>
       <c r="C200" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201">
-        <v>2936.5554972344498</v>
+        <v>2959.4443959156702</v>
       </c>
       <c r="B201">
-        <v>1.53755018343668</v>
+        <v>1.5373653041355499</v>
       </c>
       <c r="C201" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202">
-        <v>2942.81822242301</v>
+        <v>2961.4947574734301</v>
       </c>
       <c r="B202">
-        <v>1.53931438168743</v>
+        <v>1.5366411738612999</v>
       </c>
       <c r="C202" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203">
-        <v>2948.2384748854201</v>
+        <v>2438.7032634491102</v>
       </c>
       <c r="B203">
-        <v>1.53836170183641</v>
+        <v>1.19952082553013</v>
       </c>
       <c r="C203" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204">
-        <v>2952.8162546216699</v>
+        <v>2478.00031790412</v>
       </c>
       <c r="B204">
-        <v>1.5381936982922899</v>
+        <v>1.2248760489181401</v>
       </c>
       <c r="C204" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205">
-        <v>2956.5515616317498</v>
+        <v>2516.7904133812299</v>
       </c>
       <c r="B205">
-        <v>1.5379618744082899</v>
+        <v>1.24953138922889</v>
       </c>
       <c r="C205" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206">
-        <v>2959.4443959156702</v>
+        <v>2555.0735498804302</v>
       </c>
       <c r="B206">
-        <v>1.5373653041355499</v>
+        <v>1.2725331329506999</v>
       </c>
       <c r="C206" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207">
-        <v>2961.4947574734301</v>
+        <v>2592.84972740173</v>
       </c>
       <c r="B207">
-        <v>1.5366411738612999</v>
+        <v>1.2959746844889299</v>
       </c>
       <c r="C207" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208">
-        <v>2240.9857705551399</v>
+        <v>2630.1189459451198</v>
       </c>
       <c r="B208">
-        <v>1.07</v>
+        <v>1.3213709835877501</v>
       </c>
       <c r="C208" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209">
-        <v>2280.2687542798099</v>
+        <v>2666.88120551061</v>
       </c>
       <c r="B209">
-        <v>1.09568894127575</v>
+        <v>1.34337161573136</v>
       </c>
       <c r="C209" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210">
-        <v>2319.6819954315501</v>
+        <v>2703.1365060981998</v>
       </c>
       <c r="B210">
-        <v>1.12187973313379</v>
+        <v>1.36650703755018</v>
       </c>
       <c r="C210" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211">
-        <v>2359.2254940103498</v>
+        <v>2738.88484770788</v>
       </c>
       <c r="B211">
-        <v>1.14761902443993</v>
+        <v>1.3880330446984599</v>
       </c>
       <c r="C211" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212">
-        <v>2398.8992500161999</v>
+        <v>2774.1262303396602</v>
       </c>
       <c r="B212">
-        <v>1.1730188618791</v>
+        <v>1.4105271760795</v>
       </c>
       <c r="C212" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213">
-        <v>2438.7032634491102</v>
+        <v>2808.8606539935299</v>
       </c>
       <c r="B213">
-        <v>1.19952082553013</v>
+        <v>1.4315059987464001</v>
       </c>
       <c r="C213" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214">
-        <v>2478.00031790412</v>
+        <v>2842.7725535508498</v>
       </c>
       <c r="B214">
-        <v>1.2248760489181401</v>
+        <v>1.4512224023802001</v>
       </c>
       <c r="C214" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215">
-        <v>2516.7904133812299</v>
+        <v>2875.8619290116198</v>
       </c>
       <c r="B215">
-        <v>1.24953138922889</v>
+        <v>1.4699526405061001</v>
       </c>
       <c r="C215" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216">
-        <v>2555.0735498804302</v>
+        <v>2908.1287803758401</v>
       </c>
       <c r="B216">
-        <v>1.2725331329506999</v>
+        <v>1.48836345927484</v>
       </c>
       <c r="C216" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217">
-        <v>2592.84972740173</v>
+        <v>2939.5731076435</v>
       </c>
       <c r="B217">
-        <v>1.2959746844889299</v>
+        <v>1.5050137992344499</v>
       </c>
       <c r="C217" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218">
-        <v>2630.1189459451198</v>
+        <v>2970.19491081461</v>
       </c>
       <c r="B218">
-        <v>1.3213709835877501</v>
+        <v>1.5205703805106101</v>
       </c>
       <c r="C218" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219">
-        <v>2666.88120551061</v>
+        <v>2999.9941898891698</v>
       </c>
       <c r="B219">
-        <v>1.34337161573136</v>
+        <v>1.53599333246156</v>
       </c>
       <c r="C219" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220">
-        <v>2703.1365060981998</v>
+        <v>3028.9709448671802</v>
       </c>
       <c r="B220">
-        <v>1.36650703755018</v>
+        <v>1.5502442640829801</v>
       </c>
       <c r="C220" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221">
-        <v>2738.88484770788</v>
+        <v>3057.1251757486302</v>
       </c>
       <c r="B221">
-        <v>1.3880330446984599</v>
+        <v>1.5653820445026401</v>
       </c>
       <c r="C221" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222">
-        <v>2774.1262303396602</v>
+        <v>3084.45688253353</v>
       </c>
       <c r="B222">
-        <v>1.4105271760795</v>
+        <v>1.58029078146976</v>
       </c>
       <c r="C222" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223">
-        <v>2808.8606539935299</v>
+        <v>3110.9660652218799</v>
       </c>
       <c r="B223">
-        <v>1.4315059987464001</v>
+        <v>1.5931920776264601</v>
       </c>
       <c r="C223" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224">
-        <v>2842.7725535508498</v>
+        <v>3136.6206835519401</v>
       </c>
       <c r="B224">
-        <v>1.4512224023802001</v>
+        <v>1.60591840460354</v>
       </c>
       <c r="C224" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225">
-        <v>2875.8619290116198</v>
+        <v>3161.4207375237202</v>
       </c>
       <c r="B225">
-        <v>1.4699526405061001</v>
+        <v>1.61869848507267</v>
       </c>
       <c r="C225" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226">
-        <v>2908.1287803758401</v>
+        <v>3185.36622713721</v>
       </c>
       <c r="B226">
-        <v>1.48836345927484</v>
+        <v>1.6311753063844601</v>
       </c>
       <c r="C226" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227">
-        <v>2939.5731076435</v>
+        <v>3208.4571523924101</v>
       </c>
       <c r="B227">
-        <v>1.5050137992344499</v>
+        <v>1.64044236378981</v>
       </c>
       <c r="C227" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228">
-        <v>2970.19491081461</v>
+        <v>3230.69351328933</v>
       </c>
       <c r="B228">
-        <v>1.5205703805106101</v>
+        <v>1.65059479967906</v>
       </c>
       <c r="C228" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229">
-        <v>2999.9941898891698</v>
+        <v>3252.0753098279602</v>
       </c>
       <c r="B229">
-        <v>1.53599333246156</v>
+        <v>1.6615763480035399</v>
       </c>
       <c r="C229" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230">
-        <v>3028.9709448671802</v>
+        <v>3272.6025420083101</v>
       </c>
       <c r="B230">
-        <v>1.5502442640829801</v>
+        <v>1.6711567249835699</v>
       </c>
       <c r="C230" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231">
-        <v>3057.1251757486302</v>
+        <v>3292.2752098303699</v>
       </c>
       <c r="B231">
-        <v>1.5653820445026401</v>
+        <v>1.6787723917303601</v>
       </c>
       <c r="C231" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232">
-        <v>3084.45688253353</v>
+        <v>3311.09331329414</v>
       </c>
       <c r="B232">
-        <v>1.58029078146976</v>
+        <v>1.68676116654634</v>
       </c>
       <c r="C232" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233">
-        <v>3110.9660652218799</v>
+        <v>3329.0568523996199</v>
       </c>
       <c r="B233">
-        <v>1.5931920776264601</v>
+        <v>1.69456875106394</v>
       </c>
       <c r="C233" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234">
-        <v>3136.6206835519401</v>
+        <v>2441.2219080167401</v>
       </c>
       <c r="B234">
-        <v>1.60591840460354</v>
+        <v>1.1967052610144</v>
       </c>
       <c r="C234" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235">
-        <v>3161.4207375237202</v>
+        <v>2482.1522911788402</v>
       </c>
       <c r="B235">
-        <v>1.61869848507267</v>
+        <v>1.2225699748583601</v>
       </c>
       <c r="C235" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236">
-        <v>3185.36622713721</v>
+        <v>2523.3655276065401</v>
       </c>
       <c r="B236">
-        <v>1.6311753063844601</v>
+        <v>1.2480963201239399</v>
       </c>
       <c r="C236" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237">
-        <v>3208.4571523924101</v>
+        <v>2564.86161729984</v>
       </c>
       <c r="B237">
-        <v>1.64044236378981</v>
+        <v>1.2734380429364001</v>
       </c>
       <c r="C237" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238">
-        <v>3230.69351328933</v>
+        <v>2606.6405602587301</v>
       </c>
       <c r="B238">
-        <v>1.65059479967906</v>
+        <v>1.29961700799865</v>
       </c>
       <c r="C238" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239">
-        <v>3252.0753098279602</v>
+        <v>2648.7023564832102</v>
       </c>
       <c r="B239">
-        <v>1.6615763480035399</v>
+        <v>1.324407481323</v>
       </c>
       <c r="C239" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240">
-        <v>3272.6025420083101</v>
+        <v>2691.0470059732902</v>
       </c>
       <c r="B240">
-        <v>1.6711567249835699</v>
+        <v>1.3479731609657399</v>
       </c>
       <c r="C240" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241">
-        <v>3292.2752098303699</v>
+        <v>2733.6745087289701</v>
       </c>
       <c r="B241">
-        <v>1.6787723917303601</v>
+        <v>1.37232125223957</v>
       </c>
       <c r="C241" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242">
-        <v>3311.09331329414</v>
+        <v>2776.5848647502498</v>
       </c>
       <c r="B242">
-        <v>1.68676116654634</v>
+        <v>1.39957969043138</v>
       </c>
       <c r="C242" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243">
-        <v>3329.0568523996199</v>
+        <v>2819.7780740371199</v>
       </c>
       <c r="B243">
-        <v>1.69456875106394</v>
+        <v>1.4248083432262399</v>
       </c>
       <c r="C243" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244">
-        <v>2240.9818022807499</v>
+        <v>2863.25413658959</v>
       </c>
       <c r="B244">
-        <v>1.07</v>
+        <v>1.44971350548487</v>
       </c>
       <c r="C244" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245">
-        <v>2280.4303146786401</v>
+        <v>2906.8078828899302</v>
       </c>
       <c r="B245">
-        <v>1.093672513449</v>
+        <v>1.4729887604645999</v>
       </c>
       <c r="C245" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246">
-        <v>2320.17858145119</v>
+        <v>2950.4393129381701</v>
       </c>
       <c r="B246">
-        <v>1.1186899170573501</v>
+        <v>1.49621676382431</v>
       </c>
       <c r="C246" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247">
-        <v>2360.2266025983799</v>
+        <v>2994.1484267342798</v>
       </c>
       <c r="B247">
-        <v>1.14402802890893</v>
+        <v>1.5182030407014899</v>
       </c>
       <c r="C247" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248">
-        <v>2400.57437812024</v>
+        <v>3037.9352242782802</v>
       </c>
       <c r="B248">
-        <v>1.16968139295141</v>
+        <v>1.5395708727853601</v>
       </c>
       <c r="C248" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249">
-        <v>2441.2219080167401</v>
+        <v>3081.7997055701599</v>
       </c>
       <c r="B249">
-        <v>1.1967052610144</v>
+        <v>1.5608831429560699</v>
       </c>
       <c r="C249" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250">
-        <v>2482.1522911788402</v>
+        <v>3125.7418706099302</v>
       </c>
       <c r="B250">
-        <v>1.2225699748583601</v>
+        <v>1.5839000517753199</v>
       </c>
       <c r="C250" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251">
-        <v>2523.3655276065401</v>
+        <v>3169.7617193975798</v>
       </c>
       <c r="B251">
-        <v>1.2480963201239399</v>
+        <v>1.6077028430301901</v>
       </c>
       <c r="C251" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252">
-        <v>2564.86161729984</v>
+        <v>3213.85925193311</v>
       </c>
       <c r="B252">
-        <v>1.2734380429364001</v>
+        <v>1.6319651861723301</v>
       </c>
       <c r="C252" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253">
-        <v>2606.6405602587301</v>
+        <v>3258.0344682165201</v>
       </c>
       <c r="B253">
-        <v>1.29961700799865</v>
+        <v>1.6559160046383701</v>
       </c>
       <c r="C253" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254">
-        <v>2648.7023564832102</v>
+        <v>3302.2873682478198</v>
       </c>
       <c r="B254">
-        <v>1.324407481323</v>
+        <v>1.67910550919137</v>
       </c>
       <c r="C254" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255">
-        <v>2691.0470059732902</v>
+        <v>3346.46119728024</v>
       </c>
       <c r="B255">
-        <v>1.3479731609657399</v>
+        <v>1.7036997356143</v>
       </c>
       <c r="C255" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256">
-        <v>2733.6745087289701</v>
+        <v>3390.55595531379</v>
       </c>
       <c r="B256">
-        <v>1.37232125223957</v>
+        <v>1.7284459652084501</v>
       </c>
       <c r="C256" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257">
-        <v>2776.5848647502498</v>
+        <v>3434.57164234845</v>
       </c>
       <c r="B257">
-        <v>1.39957969043138</v>
+        <v>1.75347559549073</v>
       </c>
       <c r="C257" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258">
-        <v>2819.7780740371199</v>
+        <v>3478.50825838424</v>
       </c>
       <c r="B258">
-        <v>1.4248083432262399</v>
+        <v>1.7758616822067399</v>
       </c>
       <c r="C258" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259">
-        <v>2863.25413658959</v>
+        <v>3522.3658034211599</v>
       </c>
       <c r="B259">
-        <v>1.44971350548487</v>
+        <v>1.7975191950984899</v>
       </c>
       <c r="C259" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260">
-        <v>2906.8078828899302</v>
+        <v>3566.1442774591901</v>
       </c>
       <c r="B260">
-        <v>1.4729887604645999</v>
+        <v>1.8212801246436501</v>
       </c>
       <c r="C260" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261">
-        <v>2950.4393129381701</v>
+        <v>3609.8436804983598</v>
       </c>
       <c r="B261">
-        <v>1.49621676382431</v>
+        <v>1.8467276352736</v>
       </c>
       <c r="C261" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262">
-        <v>2994.1484267342798</v>
+        <v>3653.46401253864</v>
       </c>
       <c r="B262">
-        <v>1.5182030407014899</v>
+        <v>1.86850938257786</v>
       </c>
       <c r="C262" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263">
-        <v>3037.9352242782802</v>
+        <v>3697.00527358004</v>
       </c>
       <c r="B263">
-        <v>1.5395708727853601</v>
+        <v>1.8891409329591</v>
       </c>
       <c r="C263" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264">
-        <v>3081.7997055701599</v>
+        <v>3740.46746362257</v>
       </c>
       <c r="B264">
-        <v>1.5608831429560699</v>
+        <v>1.9125447026826301</v>
       </c>
       <c r="C264" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265">
-        <v>3125.7418706099302</v>
+        <v>2453.70343299974</v>
       </c>
       <c r="B265">
-        <v>1.5839000517753199</v>
+        <v>1.1958155748185699</v>
       </c>
       <c r="C265" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266">
-        <v>3169.7617193975798</v>
+        <v>2499.3154033331898</v>
       </c>
       <c r="B266">
-        <v>1.6077028430301901</v>
+        <v>1.22228178775181</v>
       </c>
       <c r="C266" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267">
-        <v>3213.85925193311</v>
+        <v>2545.7313057759002</v>
       </c>
       <c r="B267">
-        <v>1.6319651861723301</v>
+        <v>1.2483676029070001</v>
       </c>
       <c r="C267" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268">
-        <v>3258.0344682165201</v>
+        <v>2592.9511403278698</v>
       </c>
       <c r="B268">
-        <v>1.6559160046383701</v>
+        <v>1.27427346300352</v>
       </c>
       <c r="C268" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269">
-        <v>3302.2873682478198</v>
+        <v>2640.97490698912</v>
       </c>
       <c r="B269">
-        <v>1.67910550919137</v>
+        <v>1.29958539003647</v>
       </c>
       <c r="C269" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270">
-        <v>3346.46119728024</v>
+        <v>2689.8026057596298</v>
       </c>
       <c r="B270">
-        <v>1.7036997356143</v>
+        <v>1.3248405040071001</v>
       </c>
       <c r="C270" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271">
-        <v>3390.55595531379</v>
+        <v>2739.4342366394199</v>
       </c>
       <c r="B271">
-        <v>1.7284459652084501</v>
+        <v>1.35136571412966</v>
       </c>
       <c r="C271" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272">
-        <v>3434.57164234845</v>
+        <v>2789.86979962847</v>
       </c>
       <c r="B272">
-        <v>1.75347559549073</v>
+        <v>1.37889897826953</v>
       </c>
       <c r="C272" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273">
-        <v>3478.50825838424</v>
+        <v>2841.1092947267798</v>
       </c>
       <c r="B273">
-        <v>1.7758616822067399</v>
+        <v>1.4077794669022401</v>
       </c>
       <c r="C273" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274">
-        <v>3522.3658034211599</v>
+        <v>2893.1527219343702</v>
       </c>
       <c r="B274">
-        <v>1.7975191950984899</v>
+        <v>1.43587914344302</v>
       </c>
       <c r="C274" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275">
-        <v>3566.1442774591901</v>
+        <v>2946.0000812512299</v>
       </c>
       <c r="B275">
-        <v>1.8212801246436501</v>
+        <v>1.4639039205086899</v>
       </c>
       <c r="C275" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276">
-        <v>3609.8436804983598</v>
+        <v>2999.4125016191701</v>
       </c>
       <c r="B276">
-        <v>1.8467276352736</v>
+        <v>1.49305526764717</v>
       </c>
       <c r="C276" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277">
-        <v>3653.46401253864</v>
+        <v>3053.3899830382002</v>
       </c>
       <c r="B277">
-        <v>1.86850938257786</v>
+        <v>1.5219206535785601</v>
       </c>
       <c r="C277" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278">
-        <v>3697.00527358004</v>
+        <v>3107.9325255083099</v>
       </c>
       <c r="B278">
-        <v>1.8891409329591</v>
+        <v>1.55010486791617</v>
       </c>
       <c r="C278" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279">
-        <v>3740.46746362257</v>
+        <v>3163.0401290295199</v>
       </c>
       <c r="B279">
-        <v>1.9125447026826301</v>
+        <v>1.5776352101328299</v>
       </c>
       <c r="C279" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280">
-        <v>2240.9818022807499</v>
+        <v>3218.7127936018101</v>
       </c>
       <c r="B280">
-        <v>1.07</v>
+        <v>1.6054633905904001</v>
       </c>
       <c r="C280" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281">
-        <v>2281.2624163441801</v>
+        <v>3274.95051922518</v>
       </c>
       <c r="B281">
-        <v>1.0935736124719</v>
+        <v>1.63524557340947</v>
       </c>
       <c r="C281" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282">
-        <v>2322.67488644779</v>
+        <v>3331.7533058996501</v>
       </c>
       <c r="B282">
-        <v>1.1190955825928901</v>
+        <v>1.6661720377406</v>
       </c>
       <c r="C282" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283">
-        <v>2365.2192125915899</v>
+        <v>3389.1211536251999</v>
       </c>
       <c r="B283">
-        <v>1.14547610506028</v>
+        <v>1.6960045558902299</v>
       </c>
       <c r="C283" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284">
-        <v>2408.8953947755699</v>
+        <v>3447.0540624018399</v>
       </c>
       <c r="B284">
-        <v>1.17046031755272</v>
+        <v>1.7251387884304199</v>
       </c>
       <c r="C284" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285">
-        <v>2453.70343299974</v>
+        <v>3505.5520322295602</v>
       </c>
       <c r="B285">
-        <v>1.1958155748185699</v>
+        <v>1.75696499464044</v>
       </c>
       <c r="C285" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286">
-        <v>2499.3154033331898</v>
+        <v>3564.4906109367398</v>
       </c>
       <c r="B286">
-        <v>1.22228178775181</v>
+        <v>1.7907229835027401</v>
       </c>
       <c r="C286" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287">
-        <v>2545.7313057759002</v>
+        <v>3623.8697985233698</v>
       </c>
       <c r="B287">
-        <v>1.2483676029070001</v>
+        <v>1.82281948044665</v>
       </c>
       <c r="C287" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288">
-        <v>2592.9511403278698</v>
+        <v>3683.6895949894401</v>
       </c>
       <c r="B288">
-        <v>1.27427346300352</v>
+        <v>1.8518750101297501</v>
       </c>
       <c r="C288" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289">
-        <v>2640.97490698912</v>
+        <v>3743.9500003349699</v>
       </c>
       <c r="B289">
-        <v>1.29958539003647</v>
+        <v>1.8832118169598699</v>
       </c>
       <c r="C289" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290">
-        <v>2689.8026057596298</v>
+        <v>3804.65101455995</v>
       </c>
       <c r="B290">
-        <v>1.3248405040071001</v>
+        <v>1.91604351227263</v>
       </c>
       <c r="C290" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291">
-        <v>2739.4342366394199</v>
+        <v>3865.79263766438</v>
       </c>
       <c r="B291">
-        <v>1.35136571412966</v>
+        <v>1.94960770497108</v>
       </c>
       <c r="C291" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292">
-        <v>2789.86979962847</v>
+        <v>3927.3748696482498</v>
       </c>
       <c r="B292">
-        <v>1.37889897826953</v>
+        <v>1.98198417065843</v>
       </c>
       <c r="C292" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293">
-        <v>2841.1092947267798</v>
+        <v>3989.39771051158</v>
       </c>
       <c r="B293">
-        <v>1.4077794669022401</v>
+        <v>2.0128571816412699</v>
       </c>
       <c r="C293" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294">
-        <v>2893.1527219343702</v>
+        <v>4051.8611602543601</v>
       </c>
       <c r="B294">
-        <v>1.43587914344302</v>
+        <v>2.0417329332819998</v>
       </c>
       <c r="C294" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295">
-        <v>2946.0000812512299</v>
+        <v>4114.7652188765896</v>
       </c>
       <c r="B295">
-        <v>1.4639039205086899</v>
+        <v>2.0763028802100298</v>
       </c>
       <c r="C295" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296">
-        <v>2999.4125016191701</v>
+        <v>2450.4282688439398</v>
       </c>
       <c r="B296">
-        <v>1.49305526764717</v>
+        <v>1.21363933690557</v>
       </c>
       <c r="C296" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297">
-        <v>3053.3899830382002</v>
+        <v>2495.29904087458</v>
       </c>
       <c r="B297">
-        <v>1.5219206535785601</v>
+        <v>1.2433825184492699</v>
       </c>
       <c r="C297" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298">
-        <v>3107.9325255083099</v>
+        <v>2541.3282363713201</v>
       </c>
       <c r="B298">
-        <v>1.55010486791617</v>
+        <v>1.27589437277754</v>
       </c>
       <c r="C298" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299">
-        <v>3163.0401290295199</v>
+        <v>2588.5158553341898</v>
       </c>
       <c r="B299">
-        <v>1.5776352101328299</v>
+        <v>1.30671236032576</v>
       </c>
       <c r="C299" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300">
-        <v>3218.7127936018101</v>
+        <v>2636.86189776316</v>
       </c>
       <c r="B300">
-        <v>1.6054633905904001</v>
+        <v>1.33671572815488</v>
       </c>
       <c r="C300" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301">
-        <v>3274.95051922518</v>
+        <v>2686.3663636582501</v>
       </c>
       <c r="B301">
-        <v>1.63524557340947</v>
+        <v>1.3695509178175</v>
       </c>
       <c r="C301" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302">
-        <v>3331.7533058996501</v>
+        <v>2737.0292530194602</v>
       </c>
       <c r="B302">
-        <v>1.6661720377406</v>
+        <v>1.4017901925152301</v>
       </c>
       <c r="C302" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303">
-        <v>3389.1211536251999</v>
+        <v>2788.8505658467702</v>
       </c>
       <c r="B303">
-        <v>1.6960045558902299</v>
+        <v>1.43512490056797</v>
       </c>
       <c r="C303" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304">
-        <v>3447.0540624018399</v>
+        <v>2841.8303021401998</v>
       </c>
       <c r="B304">
-        <v>1.7251387884304199</v>
+        <v>1.46896170779625</v>
       </c>
       <c r="C304" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305">
-        <v>3505.5520322295602</v>
+        <v>2895.9684618997499</v>
       </c>
       <c r="B305">
-        <v>1.75696499464044</v>
+        <v>1.50354814056525</v>
       </c>
       <c r="C305" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306">
-        <v>3564.4906109367398</v>
+        <v>2951.2650451254099</v>
       </c>
       <c r="B306">
-        <v>1.7907229835027401</v>
+        <v>1.53684104309409</v>
       </c>
       <c r="C306" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307">
-        <v>3623.8697985233698</v>
+        <v>3007.9095398489399</v>
       </c>
       <c r="B307">
-        <v>1.82281948044665</v>
+        <v>1.5703515242297501</v>
       </c>
       <c r="C307" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308">
-        <v>3683.6895949894401</v>
+        <v>3065.9019460703498</v>
       </c>
       <c r="B308">
-        <v>1.8518750101297501</v>
+        <v>1.6041747241918001</v>
       </c>
       <c r="C308" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309">
-        <v>3743.9500003349699</v>
+        <v>3125.2422637896302</v>
       </c>
       <c r="B309">
-        <v>1.8832118169598699</v>
+        <v>1.63778673172398</v>
       </c>
       <c r="C309" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310">
-        <v>3804.65101455995</v>
+        <v>3185.9304930067901</v>
       </c>
       <c r="B310">
-        <v>1.91604351227263</v>
+        <v>1.67263251593663</v>
       </c>
       <c r="C310" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311">
-        <v>3865.79263766438</v>
+        <v>3247.96663372183</v>
       </c>
       <c r="B311">
-        <v>1.94960770497108</v>
+        <v>1.7075471561973199</v>
       </c>
       <c r="C311" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312">
-        <v>3927.3748696482498</v>
+        <v>3311.3506859347399</v>
       </c>
       <c r="B312">
-        <v>1.98198417065843</v>
+        <v>1.7429279573629</v>
       </c>
       <c r="C312" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313">
-        <v>3989.39771051158</v>
+        <v>3376.0826496455302</v>
       </c>
       <c r="B313">
-        <v>2.0128571816412699</v>
+        <v>1.77769758676863</v>
       </c>
       <c r="C313" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314">
-        <v>4051.8611602543601</v>
+        <v>3442.16252485419</v>
       </c>
       <c r="B314">
-        <v>2.0417329332819998</v>
+        <v>1.81369749890073</v>
       </c>
       <c r="C314" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315">
-        <v>4114.7652188765896</v>
+        <v>3509.5903115607298</v>
       </c>
       <c r="B315">
-        <v>2.0763028802100298</v>
+        <v>1.8522467714609201</v>
       </c>
       <c r="C315" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316">
-        <v>2240.9857705551399</v>
+        <v>3578.36600976515</v>
       </c>
       <c r="B316">
-        <v>1.07</v>
+        <v>1.8928535119879799</v>
       </c>
       <c r="C316" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317">
-        <v>2281.0504213061399</v>
+        <v>3648.5939601433302</v>
       </c>
       <c r="B317">
-        <v>1.09674218128339</v>
+        <v>1.9333626528054799</v>
       </c>
       <c r="C317" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318">
-        <v>2322.0269965105199</v>
+        <v>3720.2741626952902</v>
       </c>
       <c r="B318">
-        <v>1.1260511878592701</v>
+        <v>1.9712235533537601</v>
       </c>
       <c r="C318" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319">
-        <v>2363.9154961682798</v>
+        <v>3793.4066174210202</v>
       </c>
       <c r="B319">
-        <v>1.1551875717809901</v>
+        <v>2.0119212299051799</v>
       </c>
       <c r="C319" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320">
-        <v>2406.7159202794201</v>
+        <v>3867.9913243205201</v>
       </c>
       <c r="B320">
-        <v>1.18377023020687</v>
+        <v>2.0541334338674302</v>
       </c>
       <c r="C320" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321">
-        <v>2450.4282688439398</v>
+        <v>3944.0282833937999</v>
       </c>
       <c r="B321">
-        <v>1.21363933690557</v>
+        <v>2.09542973776691</v>
       </c>
       <c r="C321" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322">
-        <v>2495.29904087458</v>
+        <v>4021.5174946408501</v>
       </c>
       <c r="B322">
-        <v>1.2433825184492699</v>
+        <v>2.1374295056863599</v>
       </c>
       <c r="C322" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323">
-        <v>2541.3282363713201</v>
+        <v>4100.4589580616603</v>
       </c>
       <c r="B323">
-        <v>1.27589437277754</v>
+        <v>2.1792567370668299</v>
       </c>
       <c r="C323" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324">
-        <v>2588.5158553341898</v>
+        <v>4180.8526736562499</v>
       </c>
       <c r="B324">
-        <v>1.30671236032576</v>
+        <v>2.2206499827289501</v>
       </c>
       <c r="C324" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325">
-        <v>2636.86189776316</v>
+        <v>4262.6986414246203</v>
       </c>
       <c r="B325">
-        <v>1.33671572815488</v>
+        <v>2.2639763342631398</v>
       </c>
       <c r="C325" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326">
-        <v>2686.3663636582501</v>
+        <v>4345.9968613667497</v>
       </c>
       <c r="B326">
-        <v>1.3695509178175</v>
+        <v>2.3083468095290098</v>
       </c>
       <c r="C326" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A327">
-        <v>2737.0292530194602</v>
-      </c>
-      <c r="B327">
-        <v>1.4017901925152301</v>
-      </c>
-      <c r="C327" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A328">
-        <v>2788.8505658467702</v>
-      </c>
-      <c r="B328">
-        <v>1.43512490056797</v>
-      </c>
-      <c r="C328" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A329">
-        <v>2841.8303021401998</v>
-      </c>
-      <c r="B329">
-        <v>1.46896170779625</v>
-      </c>
-      <c r="C329" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A330">
-        <v>2895.9684618997499</v>
-      </c>
-      <c r="B330">
-        <v>1.50354814056525</v>
-      </c>
-      <c r="C330" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A331">
-        <v>2951.2650451254099</v>
-      </c>
-      <c r="B331">
-        <v>1.53684104309409</v>
-      </c>
-      <c r="C331" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A332">
-        <v>3007.9095398489399</v>
-      </c>
-      <c r="B332">
-        <v>1.5703515242297501</v>
-      </c>
-      <c r="C332" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A333">
-        <v>3065.9019460703498</v>
-      </c>
-      <c r="B333">
-        <v>1.6041747241918001</v>
-      </c>
-      <c r="C333" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A334">
-        <v>3125.2422637896302</v>
-      </c>
-      <c r="B334">
-        <v>1.63778673172398</v>
-      </c>
-      <c r="C334" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A335">
-        <v>3185.9304930067901</v>
-      </c>
-      <c r="B335">
-        <v>1.67263251593663</v>
-      </c>
-      <c r="C335" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A336">
-        <v>3247.96663372183</v>
-      </c>
-      <c r="B336">
-        <v>1.7075471561973199</v>
-      </c>
-      <c r="C336" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A337">
-        <v>3311.3506859347399</v>
-      </c>
-      <c r="B337">
-        <v>1.7429279573629</v>
-      </c>
-      <c r="C337" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A338">
-        <v>3376.0826496455302</v>
-      </c>
-      <c r="B338">
-        <v>1.77769758676863</v>
-      </c>
-      <c r="C338" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A339">
-        <v>3442.16252485419</v>
-      </c>
-      <c r="B339">
-        <v>1.81369749890073</v>
-      </c>
-      <c r="C339" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A340">
-        <v>3509.5903115607298</v>
-      </c>
-      <c r="B340">
-        <v>1.8522467714609201</v>
-      </c>
-      <c r="C340" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A341">
-        <v>3578.36600976515</v>
-      </c>
-      <c r="B341">
-        <v>1.8928535119879799</v>
-      </c>
-      <c r="C341" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A342">
-        <v>3648.5939601433302</v>
-      </c>
-      <c r="B342">
-        <v>1.9333626528054799</v>
-      </c>
-      <c r="C342" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A343">
-        <v>3720.2741626952902</v>
-      </c>
-      <c r="B343">
-        <v>1.9712235533537601</v>
-      </c>
-      <c r="C343" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A344">
-        <v>3793.4066174210202</v>
-      </c>
-      <c r="B344">
-        <v>2.0119212299051799</v>
-      </c>
-      <c r="C344" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A345">
-        <v>3867.9913243205201</v>
-      </c>
-      <c r="B345">
-        <v>2.0541334338674302</v>
-      </c>
-      <c r="C345" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A346">
-        <v>3944.0282833937999</v>
-      </c>
-      <c r="B346">
-        <v>2.09542973776691</v>
-      </c>
-      <c r="C346" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A347">
-        <v>4021.5174946408501</v>
-      </c>
-      <c r="B347">
-        <v>2.1374295056863599</v>
-      </c>
-      <c r="C347" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A348">
-        <v>4100.4589580616603</v>
-      </c>
-      <c r="B348">
-        <v>2.1792567370668299</v>
-      </c>
-      <c r="C348" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A349">
-        <v>4180.8526736562499</v>
-      </c>
-      <c r="B349">
-        <v>2.2206499827289501</v>
-      </c>
-      <c r="C349" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A350">
-        <v>4262.6986414246203</v>
-      </c>
-      <c r="B350">
-        <v>2.2639763342631398</v>
-      </c>
-      <c r="C350" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A351">
-        <v>4345.9968613667497</v>
-      </c>
-      <c r="B351">
-        <v>2.3083468095290098</v>
-      </c>
-      <c r="C351" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4962,31 +4687,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>